<commit_message>
Produces valid and EDI congruent EML for fish passage data
</commit_message>
<xml_diff>
--- a/data-raw/FISHBIO submission/FISHBIO_passage_metadata.xlsx
+++ b/data-raw/FISHBIO submission/FISHBIO_passage_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\fishbio-stanislaus-o.mykiss\data-raw\FISHBIO submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFA3B69-A614-4743-BDD2-0EE5303073FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4D3407-6563-47FA-B39B-AC7B0B55B51F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10080" yWindow="-16560" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22710" yWindow="-14745" windowWidth="24000" windowHeight="11835" tabRatio="834" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="205">
   <si>
     <t>first_name</t>
   </si>
@@ -314,9 +314,6 @@
     <t>PassageTime</t>
   </si>
   <si>
-    <t>PassageDIrection</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
@@ -356,9 +353,6 @@
     <t>VideoQuality</t>
   </si>
   <si>
-    <t>VideoProblem</t>
-  </si>
-  <si>
     <t>Date when individual was counted as passing</t>
   </si>
   <si>
@@ -380,277 +374,283 @@
     <t>nominal</t>
   </si>
   <si>
+    <t>Species of fish recorded passing the weir</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>Depth of the body measured at insertion of the dorsal fin</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>millimeter</t>
+  </si>
+  <si>
+    <t>natural</t>
+  </si>
+  <si>
+    <t>Emperical coefficient used to estimate fish length</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>Estimated total length of fish passing through the weir</t>
+  </si>
+  <si>
+    <t>Degree of maturity of recoded fish</t>
+  </si>
+  <si>
+    <t>Count of fish passing through the weir</t>
+  </si>
+  <si>
+    <t>Sex of individual if applicable</t>
+  </si>
+  <si>
+    <t>Whether or not the adipose fin has been clipped</t>
+  </si>
+  <si>
+    <t>Condition used to indicate health of passing individual</t>
+  </si>
+  <si>
+    <t>Level of certainty in species identification</t>
+  </si>
+  <si>
+    <t>Indicator of quality of counting device silhouette based identification</t>
+  </si>
+  <si>
+    <t>Indicator of quality of video image used for identification</t>
+  </si>
+  <si>
+    <t>Indicator of problems with video monitoring</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Any additional comments describing the passage record</t>
+  </si>
+  <si>
+    <t>PassageDirection</t>
+  </si>
+  <si>
+    <t>Upstream passage</t>
+  </si>
+  <si>
+    <t>Downstream passage</t>
+  </si>
+  <si>
+    <t>RBT</t>
+  </si>
+  <si>
+    <t>Rainbow trout/Steelhead</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>1+</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Age 1+</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Juvenile</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Adipose fin present, not clipped</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Adipose fin clipped</t>
+  </si>
+  <si>
+    <t>UNK</t>
+  </si>
+  <si>
+    <t>Status of adipose fin unknown</t>
+  </si>
+  <si>
+    <t>GOOD</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Whether individual was counted using counting device, trap, or temporary video</t>
+  </si>
+  <si>
+    <t>Individual was in good condition upon passage or release</t>
+  </si>
+  <si>
+    <t>Counting device was triggered by object that was not a fish</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Positive identification</t>
+  </si>
+  <si>
+    <t>VL</t>
+  </si>
+  <si>
+    <t>Identification very likely</t>
+  </si>
+  <si>
+    <t>Identification likely</t>
+  </si>
+  <si>
+    <t>Vaki sillouette clearly shows fish outline</t>
+  </si>
+  <si>
+    <t>Vaki sillouette partially shows fish outline</t>
+  </si>
+  <si>
+    <t>Vaki sillouette is very distorted</t>
+  </si>
+  <si>
+    <t>No Vaki sillouette available</t>
+  </si>
+  <si>
+    <t>FAIR</t>
+  </si>
+  <si>
+    <t>POOR</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>Video image clear</t>
+  </si>
+  <si>
+    <t>Video image partially obscured or low light</t>
+  </si>
+  <si>
+    <t>Video image cloud and obscured or insufficient light</t>
+  </si>
+  <si>
+    <t>No video image available</t>
+  </si>
+  <si>
+    <t>VideoProblems</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Kelt</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Sex undetermined</t>
+  </si>
+  <si>
+    <t>Debris obscuring the frame</t>
+  </si>
+  <si>
+    <t>Equipment malfunctioning</t>
+  </si>
+  <si>
+    <t>Multiple individuals passing at the same time</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Not applicable, no problem</t>
+  </si>
+  <si>
+    <t>No passage in frame</t>
+  </si>
+  <si>
+    <t>Orientation of frame is misaligned</t>
+  </si>
+  <si>
+    <t>Split screen problem</t>
+  </si>
+  <si>
+    <t>Turbidity obscuring the frame</t>
+  </si>
+  <si>
+    <t>annually</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>CVPIA</t>
+  </si>
+  <si>
+    <t>enumerated</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>DOWN</t>
+  </si>
+  <si>
+    <t>NO FISH</t>
+  </si>
+  <si>
     <t>text</t>
-  </si>
-  <si>
-    <t>Species of fish recorded passing the weir</t>
-  </si>
-  <si>
-    <t>ratio</t>
-  </si>
-  <si>
-    <t>Depth of the body measured at insertion of the dorsal fin</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>millimeter</t>
-  </si>
-  <si>
-    <t>natural</t>
-  </si>
-  <si>
-    <t>Emperical coefficient used to estimate fish length</t>
-  </si>
-  <si>
-    <t>dimensionless</t>
-  </si>
-  <si>
-    <t>real</t>
-  </si>
-  <si>
-    <t>Estimated total length of fish passing through the weir</t>
-  </si>
-  <si>
-    <t>Degree of maturity of recoded fish</t>
-  </si>
-  <si>
-    <t>Count of fish passing through the weir</t>
-  </si>
-  <si>
-    <t>Sex of individual if applicable</t>
-  </si>
-  <si>
-    <t>Whether or not the adipose fin has been clipped</t>
-  </si>
-  <si>
-    <t>Condition used to indicate health of passing individual</t>
-  </si>
-  <si>
-    <t>Level of certainty in species identification</t>
-  </si>
-  <si>
-    <t>Indicator of quality of counting device silhouette based identification</t>
-  </si>
-  <si>
-    <t>Indicator of quality of video image used for identification</t>
-  </si>
-  <si>
-    <t>Indicator of problems with video monitoring</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Any additional comments describing the passage record</t>
-  </si>
-  <si>
-    <t>PassageDirection</t>
-  </si>
-  <si>
-    <t>Up</t>
-  </si>
-  <si>
-    <t>Down</t>
-  </si>
-  <si>
-    <t>Upstream passage</t>
-  </si>
-  <si>
-    <t>Downstream passage</t>
-  </si>
-  <si>
-    <t>RBT</t>
-  </si>
-  <si>
-    <t>Rainbow trout/Steelhead</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>1+</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>Age 1+</t>
-  </si>
-  <si>
-    <t>Adult</t>
-  </si>
-  <si>
-    <t>Juvenile</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Adipose fin present, not clipped</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Adipose fin clipped</t>
-  </si>
-  <si>
-    <t>UNK</t>
-  </si>
-  <si>
-    <t>Status of adipose fin unknown</t>
-  </si>
-  <si>
-    <t>GOOD</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>Whether individual was counted using counting device, trap, or temporary video</t>
-  </si>
-  <si>
-    <t>Individual was in good condition upon passage or release</t>
-  </si>
-  <si>
-    <t>No Fish</t>
-  </si>
-  <si>
-    <t>Counting device was triggered by object that was not a fish</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Positive identification</t>
-  </si>
-  <si>
-    <t>VL</t>
-  </si>
-  <si>
-    <t>Identification very likely</t>
-  </si>
-  <si>
-    <t>Identification likely</t>
-  </si>
-  <si>
-    <t>Vaki sillouette clearly shows fish outline</t>
-  </si>
-  <si>
-    <t>Vaki sillouette partially shows fish outline</t>
-  </si>
-  <si>
-    <t>Vaki sillouette is very distorted</t>
-  </si>
-  <si>
-    <t>No Vaki sillouette available</t>
-  </si>
-  <si>
-    <t>FAIR</t>
-  </si>
-  <si>
-    <t>POOR</t>
-  </si>
-  <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>Video image clear</t>
-  </si>
-  <si>
-    <t>Video image partially obscured or low light</t>
-  </si>
-  <si>
-    <t>Video image cloud and obscured or insufficient light</t>
-  </si>
-  <si>
-    <t>No video image available</t>
-  </si>
-  <si>
-    <t>VideoProblems</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>EM</t>
-  </si>
-  <si>
-    <t>MP</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>SS</t>
-  </si>
-  <si>
-    <t>TB</t>
-  </si>
-  <si>
-    <t>ordinal</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>Kelt</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Sex undetermined</t>
-  </si>
-  <si>
-    <t>Debris obscuring the frame</t>
-  </si>
-  <si>
-    <t>Equipment malfunctioning</t>
-  </si>
-  <si>
-    <t>Multiple individuals passing at the same time</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Not applicable, no problem</t>
-  </si>
-  <si>
-    <t>No passage in frame</t>
-  </si>
-  <si>
-    <t>Orientation of frame is misaligned</t>
-  </si>
-  <si>
-    <t>Split screen problem</t>
-  </si>
-  <si>
-    <t>Turbidity obscuring the frame</t>
-  </si>
-  <si>
-    <t>annually</t>
-  </si>
-  <si>
-    <t>integer</t>
   </si>
 </sst>
 </file>
@@ -1255,9 +1255,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMH19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1325,22 +1325,22 @@
     </row>
     <row r="2" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="L2" t="s">
         <v>108</v>
-      </c>
-      <c r="K2" t="s">
-        <v>110</v>
-      </c>
-      <c r="L2" t="s">
-        <v>110</v>
       </c>
       <c r="M2" s="14">
         <v>38361</v>
@@ -1354,72 +1354,72 @@
         <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K3" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>111</v>
-      </c>
       <c r="L3" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M3" s="16"/>
       <c r="N3" s="17"/>
     </row>
     <row r="4" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>92</v>
+      <c r="A4" t="s">
+        <v>133</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="M6" s="2">
         <v>1</v>
@@ -1430,25 +1430,25 @@
     </row>
     <row r="7" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="M7" s="2">
         <v>0.01</v>
@@ -1459,25 +1459,25 @@
     </row>
     <row r="8" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="M8" s="2">
         <v>1</v>
@@ -1488,39 +1488,39 @@
     </row>
     <row r="9" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="M10" s="2">
         <v>-1</v>
@@ -1531,128 +1531,128 @@
     </row>
     <row r="11" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>106</v>
+        <v>172</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>114</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>114</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1687,8 +1687,8 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1711,376 +1711,376 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B10" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B11" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B12" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B14" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B23" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B26" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B27" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B28" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B30" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B31" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B33" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B34" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B35" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2230,7 +2230,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -2273,6 +2273,11 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2492,7 +2497,7 @@
         <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2517,7 +2522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>